<commit_message>
MenB change to lower minimum age
</commit_message>
<xml_diff>
--- a/schedules/MeningococcalB.xlsx
+++ b/schedules/MeningococcalB.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\IMMUN\Claire\Forecaster\Mening B\12.28.17 forecaster document copies\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10845" windowHeight="7785" tabRatio="242"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18285" windowHeight="9675" tabRatio="242"/>
   </bookViews>
   <sheets>
     <sheet name="Schedules" sheetId="1" r:id="rId1"/>
@@ -13,12 +18,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Schedules!$A$1:$I$241</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="71">
   <si>
     <t>Forecast Series Name</t>
   </si>
@@ -268,12 +273,15 @@
   <si>
     <t>Greater Than 6 Months</t>
   </si>
+  <si>
+    <t>10 years</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -591,9 +599,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -601,6 +606,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -707,17 +715,23 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>200024</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>146126</xdr:rowOff>
+      <xdr:rowOff>146125</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="MenB 2-dose 3_7_2017 - MenB.png"/>
+        <xdr:cNvPr id="4" name="Picture 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -725,7 +739,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="104774" y="1076325"/>
-          <a:ext cx="7553325" cy="6137351"/>
+          <a:ext cx="7553325" cy="6137350"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1018,7 +1032,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1060,7 +1074,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1077,19 +1091,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I239"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J54" sqref="J54"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
@@ -1099,8 +1115,8 @@
     <col min="10" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="8.25" customHeight="1"/>
-    <row r="2" spans="2:9">
+    <row r="1" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1108,14 +1124,14 @@
       <c r="D2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-    </row>
-    <row r="3" spans="2:9">
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
         <v>53</v>
       </c>
@@ -1134,7 +1150,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:9">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
         <v>33</v>
       </c>
@@ -1153,7 +1169,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="5" spans="2:9">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="10" t="s">
         <v>34</v>
       </c>
@@ -1172,7 +1188,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="23" t="s">
         <v>37</v>
       </c>
@@ -1187,67 +1203,67 @@
       <c r="H6" s="10"/>
       <c r="I6" s="9"/>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8"/>
     </row>
-    <row r="25" spans="5:5">
+    <row r="25" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E25" s="13"/>
     </row>
-    <row r="26" spans="5:5">
+    <row r="26" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E26" s="13"/>
     </row>
-    <row r="27" spans="5:5">
+    <row r="27" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E27" s="13"/>
     </row>
-    <row r="28" spans="5:5">
+    <row r="28" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E28" s="13"/>
     </row>
-    <row r="29" spans="5:5">
+    <row r="29" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E29" s="13"/>
     </row>
-    <row r="30" spans="5:5">
+    <row r="30" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E30" s="13"/>
     </row>
-    <row r="31" spans="5:5">
+    <row r="31" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E31" s="13"/>
     </row>
-    <row r="32" spans="5:5">
+    <row r="32" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E32" s="13"/>
     </row>
-    <row r="33" spans="2:5">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E33" s="13"/>
     </row>
-    <row r="34" spans="2:5">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E34" s="13"/>
     </row>
-    <row r="35" spans="2:5">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E35" s="13"/>
     </row>
-    <row r="36" spans="2:5">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E36" s="13"/>
     </row>
-    <row r="37" spans="2:5">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E37" s="13"/>
     </row>
-    <row r="38" spans="2:5">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E38" s="13"/>
     </row>
-    <row r="39" spans="2:5">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E39" s="13"/>
     </row>
-    <row r="40" spans="2:5">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E40" s="13"/>
     </row>
-    <row r="41" spans="2:5">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E41" s="13"/>
     </row>
-    <row r="42" spans="2:5">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E42" s="13"/>
     </row>
-    <row r="43" spans="2:5">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E43" s="13"/>
     </row>
-    <row r="47" spans="2:5" ht="14.25">
+    <row r="47" spans="2:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B47" s="5" t="s">
         <v>6</v>
       </c>
@@ -1261,7 +1277,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="2:5">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B48" s="14" t="s">
         <v>41</v>
       </c>
@@ -1272,15 +1288,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="2:5">
-      <c r="B49" s="41" t="s">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B49" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="C49" s="42"/>
-      <c r="D49" s="42"/>
-      <c r="E49" s="43"/>
-    </row>
-    <row r="50" spans="2:5">
+      <c r="C49" s="41"/>
+      <c r="D49" s="41"/>
+      <c r="E49" s="42"/>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B50" s="15"/>
       <c r="C50" s="6" t="s">
         <v>12</v>
@@ -1292,19 +1308,19 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="2:5">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B51" s="16" t="s">
         <v>15</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="D51" s="9"/>
       <c r="E51" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="2:5">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B52" s="16" t="s">
         <v>18</v>
       </c>
@@ -1312,7 +1328,7 @@
       <c r="D52" s="9"/>
       <c r="E52" s="9"/>
     </row>
-    <row r="53" spans="2:5">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B53" s="16" t="s">
         <v>19</v>
       </c>
@@ -1322,7 +1338,7 @@
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
     </row>
-    <row r="54" spans="2:5">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B54" s="16" t="s">
         <v>21</v>
       </c>
@@ -1332,7 +1348,7 @@
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
     </row>
-    <row r="55" spans="2:5">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B55" s="16" t="s">
         <v>22</v>
       </c>
@@ -1342,7 +1358,7 @@
       <c r="D55" s="9"/>
       <c r="E55" s="9"/>
     </row>
-    <row r="56" spans="2:5">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B56" s="16" t="s">
         <v>23</v>
       </c>
@@ -1352,7 +1368,7 @@
       </c>
       <c r="E56" s="9"/>
     </row>
-    <row r="57" spans="2:5">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B57" s="16" t="s">
         <v>24</v>
       </c>
@@ -1360,14 +1376,14 @@
       <c r="D57" s="9"/>
       <c r="E57" s="9"/>
     </row>
-    <row r="58" spans="2:5">
-      <c r="B58" s="40" t="s">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B58" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="C58" s="40"/>
-      <c r="D58" s="40"/>
-    </row>
-    <row r="59" spans="2:5">
+      <c r="C58" s="43"/>
+      <c r="D58" s="43"/>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B59" s="6" t="s">
         <v>3</v>
       </c>
@@ -1381,7 +1397,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="2:5">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B60" s="9" t="s">
         <v>33</v>
       </c>
@@ -1391,7 +1407,7 @@
       <c r="D60" s="18"/>
       <c r="E60" s="18"/>
     </row>
-    <row r="61" spans="2:5">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B61" s="9" t="s">
         <v>34</v>
       </c>
@@ -1401,7 +1417,7 @@
       <c r="D61" s="9"/>
       <c r="E61" s="18"/>
     </row>
-    <row r="62" spans="2:5">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B62" s="16" t="s">
         <v>28</v>
       </c>
@@ -1409,7 +1425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:5">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B63" s="16" t="s">
         <v>29</v>
       </c>
@@ -1417,7 +1433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="2:5" ht="14.25">
+    <row r="65" spans="2:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B65" s="21" t="s">
         <v>6</v>
       </c>
@@ -1429,7 +1445,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="2:5">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B66" s="14" t="s">
         <v>39</v>
       </c>
@@ -1437,15 +1453,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="2:5">
-      <c r="B67" s="40" t="s">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B67" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C67" s="40"/>
-      <c r="D67" s="40"/>
-      <c r="E67" s="40"/>
-    </row>
-    <row r="68" spans="2:5">
+      <c r="C67" s="43"/>
+      <c r="D67" s="43"/>
+      <c r="E67" s="43"/>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B68" s="15"/>
       <c r="C68" s="6" t="s">
         <v>12</v>
@@ -1457,7 +1473,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="69" spans="2:5" ht="12" customHeight="1">
+    <row r="69" spans="2:5" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B69" s="16" t="s">
         <v>15</v>
       </c>
@@ -1469,7 +1485,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="70" spans="2:5">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B70" s="16" t="s">
         <v>18</v>
       </c>
@@ -1477,7 +1493,7 @@
       <c r="D70" s="9"/>
       <c r="E70" s="9"/>
     </row>
-    <row r="71" spans="2:5">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B71" s="16" t="s">
         <v>19</v>
       </c>
@@ -1487,7 +1503,7 @@
       </c>
       <c r="E71" s="9"/>
     </row>
-    <row r="72" spans="2:5">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B72" s="16" t="s">
         <v>21</v>
       </c>
@@ -1497,7 +1513,7 @@
       </c>
       <c r="E72" s="9"/>
     </row>
-    <row r="73" spans="2:5">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B73" s="16" t="s">
         <v>22</v>
       </c>
@@ -1507,7 +1523,7 @@
       <c r="D73" s="9"/>
       <c r="E73" s="9"/>
     </row>
-    <row r="74" spans="2:5">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B74" s="16" t="s">
         <v>23</v>
       </c>
@@ -1515,7 +1531,7 @@
       <c r="D74" s="9"/>
       <c r="E74" s="9"/>
     </row>
-    <row r="75" spans="2:5">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B75" s="16" t="s">
         <v>24</v>
       </c>
@@ -1523,7 +1539,7 @@
       <c r="D75" s="9"/>
       <c r="E75" s="9"/>
     </row>
-    <row r="76" spans="2:5">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B76" s="16" t="s">
         <v>54</v>
       </c>
@@ -1531,14 +1547,14 @@
         <v>56</v>
       </c>
     </row>
-    <row r="77" spans="2:5">
-      <c r="B77" s="40" t="s">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B77" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="C77" s="40"/>
-      <c r="D77" s="40"/>
-    </row>
-    <row r="78" spans="2:5">
+      <c r="C77" s="43"/>
+      <c r="D77" s="43"/>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B78" s="6" t="s">
         <v>3</v>
       </c>
@@ -1552,7 +1568,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="2:5">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B79" s="9" t="s">
         <v>33</v>
       </c>
@@ -1562,7 +1578,7 @@
       <c r="D79" s="9"/>
       <c r="E79" s="18"/>
     </row>
-    <row r="80" spans="2:5">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B80" s="9" t="s">
         <v>34</v>
       </c>
@@ -1572,7 +1588,7 @@
       <c r="D80" s="9"/>
       <c r="E80" s="9"/>
     </row>
-    <row r="81" spans="2:5">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B81" s="16" t="s">
         <v>28</v>
       </c>
@@ -1580,7 +1596,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="2:5">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B82" s="16" t="s">
         <v>29</v>
       </c>
@@ -1588,7 +1604,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="2:5" ht="14.25">
+    <row r="84" spans="2:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B84" s="5" t="s">
         <v>6</v>
       </c>
@@ -1602,7 +1618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="2:5">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B85" s="14" t="s">
         <v>43</v>
       </c>
@@ -1611,15 +1627,15 @@
       </c>
       <c r="D85" s="14"/>
     </row>
-    <row r="86" spans="2:5">
-      <c r="B86" s="41" t="s">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B86" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="C86" s="42"/>
-      <c r="D86" s="42"/>
-      <c r="E86" s="43"/>
-    </row>
-    <row r="87" spans="2:5">
+      <c r="C86" s="41"/>
+      <c r="D86" s="41"/>
+      <c r="E86" s="42"/>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B87" s="15"/>
       <c r="C87" s="6" t="s">
         <v>12</v>
@@ -1631,7 +1647,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="88" spans="2:5">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B88" s="16" t="s">
         <v>15</v>
       </c>
@@ -1643,7 +1659,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="89" spans="2:5">
+    <row r="89" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B89" s="16" t="s">
         <v>18</v>
       </c>
@@ -1651,7 +1667,7 @@
       <c r="D89" s="9"/>
       <c r="E89" s="9"/>
     </row>
-    <row r="90" spans="2:5">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B90" s="16" t="s">
         <v>19</v>
       </c>
@@ -1661,7 +1677,7 @@
       </c>
       <c r="E90" s="9"/>
     </row>
-    <row r="91" spans="2:5">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B91" s="16" t="s">
         <v>21</v>
       </c>
@@ -1671,7 +1687,7 @@
       </c>
       <c r="E91" s="9"/>
     </row>
-    <row r="92" spans="2:5">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B92" s="16" t="s">
         <v>22</v>
       </c>
@@ -1681,7 +1697,7 @@
       <c r="D92" s="9"/>
       <c r="E92" s="9"/>
     </row>
-    <row r="93" spans="2:5">
+    <row r="93" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B93" s="16" t="s">
         <v>23</v>
       </c>
@@ -1689,7 +1705,7 @@
       <c r="D93" s="9"/>
       <c r="E93" s="9"/>
     </row>
-    <row r="94" spans="2:5">
+    <row r="94" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B94" s="16" t="s">
         <v>24</v>
       </c>
@@ -1697,7 +1713,7 @@
       <c r="D94" s="9"/>
       <c r="E94" s="9"/>
     </row>
-    <row r="95" spans="2:5">
+    <row r="95" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B95" s="16" t="s">
         <v>54</v>
       </c>
@@ -1705,14 +1721,14 @@
         <v>55</v>
       </c>
     </row>
-    <row r="96" spans="2:5">
-      <c r="B96" s="40" t="s">
+    <row r="96" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B96" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="C96" s="40"/>
-      <c r="D96" s="40"/>
-    </row>
-    <row r="97" spans="1:5">
+      <c r="C96" s="43"/>
+      <c r="D96" s="43"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B97" s="6" t="s">
         <v>3</v>
       </c>
@@ -1726,7 +1742,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B98" s="9" t="s">
         <v>34</v>
       </c>
@@ -1736,7 +1752,7 @@
       <c r="D98" s="9"/>
       <c r="E98" s="18"/>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B99" s="9" t="s">
         <v>33</v>
       </c>
@@ -1746,7 +1762,7 @@
       <c r="D99" s="9"/>
       <c r="E99" s="9"/>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B100" s="16" t="s">
         <v>28</v>
       </c>
@@ -1754,7 +1770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B101" s="16" t="s">
         <v>29</v>
       </c>
@@ -1762,7 +1778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="14.25">
+    <row r="103" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A103"/>
       <c r="B103" s="31" t="s">
         <v>6</v>
@@ -1777,7 +1793,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B104" s="14" t="s">
         <v>59</v>
       </c>
@@ -1786,15 +1802,15 @@
       </c>
       <c r="D104" s="14"/>
     </row>
-    <row r="105" spans="1:5">
-      <c r="B105" s="41" t="s">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B105" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="C105" s="42"/>
-      <c r="D105" s="42"/>
-      <c r="E105" s="43"/>
-    </row>
-    <row r="106" spans="1:5">
+      <c r="C105" s="41"/>
+      <c r="D105" s="41"/>
+      <c r="E105" s="42"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B106" s="15"/>
       <c r="C106" s="6" t="s">
         <v>12</v>
@@ -1806,7 +1822,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B107" s="16" t="s">
         <v>15</v>
       </c>
@@ -1818,7 +1834,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B108" s="16" t="s">
         <v>18</v>
       </c>
@@ -1826,7 +1842,7 @@
       <c r="D108" s="9"/>
       <c r="E108" s="9"/>
     </row>
-    <row r="109" spans="1:5">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B109" s="16" t="s">
         <v>19</v>
       </c>
@@ -1836,7 +1852,7 @@
       </c>
       <c r="E109" s="9"/>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B110" s="16" t="s">
         <v>21</v>
       </c>
@@ -1846,7 +1862,7 @@
       </c>
       <c r="E110" s="9"/>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B111" s="16" t="s">
         <v>22</v>
       </c>
@@ -1856,7 +1872,7 @@
       <c r="D111" s="9"/>
       <c r="E111" s="9"/>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B112" s="16" t="s">
         <v>23</v>
       </c>
@@ -1864,7 +1880,7 @@
       <c r="D112" s="9"/>
       <c r="E112" s="9"/>
     </row>
-    <row r="113" spans="2:5">
+    <row r="113" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B113" s="16" t="s">
         <v>24</v>
       </c>
@@ -1874,7 +1890,7 @@
       </c>
       <c r="E113" s="9"/>
     </row>
-    <row r="114" spans="2:5">
+    <row r="114" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B114" s="16" t="s">
         <v>54</v>
       </c>
@@ -1882,14 +1898,14 @@
         <v>56</v>
       </c>
     </row>
-    <row r="115" spans="2:5">
-      <c r="B115" s="41" t="s">
+    <row r="115" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B115" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C115" s="42"/>
-      <c r="D115" s="43"/>
-    </row>
-    <row r="116" spans="2:5">
+      <c r="C115" s="41"/>
+      <c r="D115" s="42"/>
+    </row>
+    <row r="116" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B116" s="6" t="s">
         <v>3</v>
       </c>
@@ -1903,7 +1919,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="117" spans="2:5">
+    <row r="117" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B117" s="9" t="s">
         <v>33</v>
       </c>
@@ -1913,7 +1929,7 @@
       <c r="D117" s="18"/>
       <c r="E117" s="18"/>
     </row>
-    <row r="118" spans="2:5">
+    <row r="118" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B118" s="9" t="s">
         <v>34</v>
       </c>
@@ -1923,7 +1939,7 @@
       <c r="D118" s="18"/>
       <c r="E118" s="18"/>
     </row>
-    <row r="119" spans="2:5">
+    <row r="119" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B119" s="16" t="s">
         <v>28</v>
       </c>
@@ -1931,7 +1947,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="2:5">
+    <row r="120" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B120" s="16" t="s">
         <v>29</v>
       </c>
@@ -1939,24 +1955,24 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="2:5">
+    <row r="122" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B122" s="32" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="123" spans="2:5">
+    <row r="123" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B123" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="124" spans="2:5">
-      <c r="B124" s="40" t="s">
+    <row r="124" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B124" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="C124" s="40"/>
-      <c r="D124" s="40"/>
-    </row>
-    <row r="125" spans="2:5">
+      <c r="C124" s="43"/>
+      <c r="D124" s="43"/>
+    </row>
+    <row r="125" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B125" s="35" t="s">
         <v>50</v>
       </c>
@@ -1965,14 +1981,14 @@
         <v>34</v>
       </c>
     </row>
-    <row r="126" spans="2:5">
-      <c r="B126" s="40" t="s">
+    <row r="126" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B126" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="C126" s="40"/>
-      <c r="D126" s="40"/>
-    </row>
-    <row r="127" spans="2:5">
+      <c r="C126" s="43"/>
+      <c r="D126" s="43"/>
+    </row>
+    <row r="127" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B127" s="44" t="s">
         <v>69</v>
       </c>
@@ -1981,7 +1997,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="128" spans="2:5">
+    <row r="128" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B128" s="44" t="s">
         <v>68</v>
       </c>
@@ -1990,24 +2006,24 @@
         <v>59</v>
       </c>
     </row>
-    <row r="130" spans="2:4">
+    <row r="130" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B130" s="32" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="131" spans="2:4">
+    <row r="131" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B131" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="132" spans="2:4">
-      <c r="B132" s="40" t="s">
+    <row r="132" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B132" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="C132" s="40"/>
-      <c r="D132" s="40"/>
-    </row>
-    <row r="133" spans="2:4">
+      <c r="C132" s="43"/>
+      <c r="D132" s="43"/>
+    </row>
+    <row r="133" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B133" s="33" t="s">
         <v>50</v>
       </c>
@@ -2016,14 +2032,14 @@
         <v>34</v>
       </c>
     </row>
-    <row r="134" spans="2:4">
-      <c r="B134" s="40" t="s">
+    <row r="134" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B134" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="C134" s="40"/>
-      <c r="D134" s="40"/>
-    </row>
-    <row r="135" spans="2:4">
+      <c r="C134" s="43"/>
+      <c r="D134" s="43"/>
+    </row>
+    <row r="135" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B135" s="44" t="s">
         <v>69</v>
       </c>
@@ -2032,7 +2048,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="136" spans="2:4">
+    <row r="136" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B136" s="44" t="s">
         <v>68</v>
       </c>
@@ -2041,24 +2057,24 @@
         <v>64</v>
       </c>
     </row>
-    <row r="138" spans="2:4">
+    <row r="138" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B138" s="37" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="139" spans="2:4">
+    <row r="139" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B139" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="140" spans="2:4">
-      <c r="B140" s="40" t="s">
+    <row r="140" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B140" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="C140" s="40"/>
-      <c r="D140" s="40"/>
-    </row>
-    <row r="141" spans="2:4">
+      <c r="C140" s="43"/>
+      <c r="D140" s="43"/>
+    </row>
+    <row r="141" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B141" s="38" t="s">
         <v>50</v>
       </c>
@@ -2067,14 +2083,14 @@
         <v>34</v>
       </c>
     </row>
-    <row r="142" spans="2:4">
-      <c r="B142" s="40" t="s">
+    <row r="142" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B142" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="C142" s="40"/>
-      <c r="D142" s="40"/>
-    </row>
-    <row r="143" spans="2:4">
+      <c r="C142" s="43"/>
+      <c r="D142" s="43"/>
+    </row>
+    <row r="143" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B143" s="44" t="s">
         <v>69</v>
       </c>
@@ -2083,7 +2099,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="144" spans="2:4">
+    <row r="144" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B144" s="44" t="s">
         <v>68</v>
       </c>
@@ -2092,7 +2108,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="146" spans="2:5" ht="14.25">
+    <row r="146" spans="2:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B146" s="24" t="s">
         <v>6</v>
       </c>
@@ -2106,7 +2122,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="147" spans="2:5">
+    <row r="147" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B147" s="14" t="s">
         <v>61</v>
       </c>
@@ -2115,15 +2131,15 @@
       </c>
       <c r="D147" s="14"/>
     </row>
-    <row r="148" spans="2:5">
-      <c r="B148" s="41" t="s">
+    <row r="148" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B148" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="C148" s="42"/>
-      <c r="D148" s="42"/>
-      <c r="E148" s="43"/>
-    </row>
-    <row r="149" spans="2:5">
+      <c r="C148" s="41"/>
+      <c r="D148" s="41"/>
+      <c r="E148" s="42"/>
+    </row>
+    <row r="149" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B149" s="15"/>
       <c r="C149" s="6" t="s">
         <v>12</v>
@@ -2135,7 +2151,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="150" spans="2:5">
+    <row r="150" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B150" s="16" t="s">
         <v>15</v>
       </c>
@@ -2147,7 +2163,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="151" spans="2:5">
+    <row r="151" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B151" s="16" t="s">
         <v>18</v>
       </c>
@@ -2155,7 +2171,7 @@
       <c r="D151" s="9"/>
       <c r="E151" s="9"/>
     </row>
-    <row r="152" spans="2:5">
+    <row r="152" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B152" s="16" t="s">
         <v>19</v>
       </c>
@@ -2165,7 +2181,7 @@
       </c>
       <c r="E152" s="9"/>
     </row>
-    <row r="153" spans="2:5">
+    <row r="153" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B153" s="16" t="s">
         <v>21</v>
       </c>
@@ -2175,7 +2191,7 @@
       </c>
       <c r="E153" s="9"/>
     </row>
-    <row r="154" spans="2:5">
+    <row r="154" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B154" s="16" t="s">
         <v>22</v>
       </c>
@@ -2185,7 +2201,7 @@
       <c r="D154" s="9"/>
       <c r="E154" s="9"/>
     </row>
-    <row r="155" spans="2:5">
+    <row r="155" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B155" s="16" t="s">
         <v>23</v>
       </c>
@@ -2193,7 +2209,7 @@
       <c r="D155" s="9"/>
       <c r="E155" s="9"/>
     </row>
-    <row r="156" spans="2:5">
+    <row r="156" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B156" s="16" t="s">
         <v>24</v>
       </c>
@@ -2201,7 +2217,7 @@
       <c r="D156" s="9"/>
       <c r="E156" s="9"/>
     </row>
-    <row r="157" spans="2:5">
+    <row r="157" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B157" s="16" t="s">
         <v>54</v>
       </c>
@@ -2209,14 +2225,14 @@
         <v>55</v>
       </c>
     </row>
-    <row r="158" spans="2:5">
-      <c r="B158" s="40" t="s">
+    <row r="158" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B158" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="C158" s="40"/>
-      <c r="D158" s="40"/>
-    </row>
-    <row r="159" spans="2:5">
+      <c r="C158" s="43"/>
+      <c r="D158" s="43"/>
+    </row>
+    <row r="159" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B159" s="6" t="s">
         <v>3</v>
       </c>
@@ -2230,7 +2246,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="160" spans="2:5">
+    <row r="160" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B160" s="9" t="s">
         <v>34</v>
       </c>
@@ -2240,7 +2256,7 @@
       <c r="D160" s="9"/>
       <c r="E160" s="9"/>
     </row>
-    <row r="161" spans="2:5">
+    <row r="161" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B161" s="9" t="s">
         <v>33</v>
       </c>
@@ -2250,7 +2266,7 @@
       <c r="D161" s="9"/>
       <c r="E161" s="9"/>
     </row>
-    <row r="162" spans="2:5">
+    <row r="162" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B162" s="16" t="s">
         <v>28</v>
       </c>
@@ -2258,7 +2274,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="163" spans="2:5">
+    <row r="163" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B163" s="16" t="s">
         <v>29</v>
       </c>
@@ -2266,7 +2282,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="165" spans="2:5" ht="14.25">
+    <row r="165" spans="2:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B165" s="37" t="s">
         <v>6</v>
       </c>
@@ -2280,7 +2296,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="166" spans="2:5">
+    <row r="166" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B166" s="14" t="s">
         <v>64</v>
       </c>
@@ -2289,15 +2305,15 @@
       </c>
       <c r="D166" s="14"/>
     </row>
-    <row r="167" spans="2:5">
-      <c r="B167" s="41" t="s">
+    <row r="167" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B167" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="C167" s="42"/>
-      <c r="D167" s="42"/>
-      <c r="E167" s="43"/>
-    </row>
-    <row r="168" spans="2:5">
+      <c r="C167" s="41"/>
+      <c r="D167" s="41"/>
+      <c r="E167" s="42"/>
+    </row>
+    <row r="168" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B168" s="15"/>
       <c r="C168" s="6" t="s">
         <v>12</v>
@@ -2309,7 +2325,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="169" spans="2:5">
+    <row r="169" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B169" s="16" t="s">
         <v>15</v>
       </c>
@@ -2321,7 +2337,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" spans="2:5">
+    <row r="170" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B170" s="16" t="s">
         <v>18</v>
       </c>
@@ -2329,7 +2345,7 @@
       <c r="D170" s="9"/>
       <c r="E170" s="9"/>
     </row>
-    <row r="171" spans="2:5">
+    <row r="171" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B171" s="16" t="s">
         <v>19</v>
       </c>
@@ -2339,7 +2355,7 @@
       </c>
       <c r="E171" s="9"/>
     </row>
-    <row r="172" spans="2:5">
+    <row r="172" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B172" s="16" t="s">
         <v>21</v>
       </c>
@@ -2349,7 +2365,7 @@
       </c>
       <c r="E172" s="9"/>
     </row>
-    <row r="173" spans="2:5">
+    <row r="173" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B173" s="16" t="s">
         <v>22</v>
       </c>
@@ -2359,7 +2375,7 @@
       <c r="D173" s="9"/>
       <c r="E173" s="9"/>
     </row>
-    <row r="174" spans="2:5">
+    <row r="174" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B174" s="16" t="s">
         <v>23</v>
       </c>
@@ -2367,7 +2383,7 @@
       <c r="D174" s="9"/>
       <c r="E174" s="9"/>
     </row>
-    <row r="175" spans="2:5">
+    <row r="175" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B175" s="16" t="s">
         <v>24</v>
       </c>
@@ -2377,7 +2393,7 @@
       </c>
       <c r="E175" s="9"/>
     </row>
-    <row r="176" spans="2:5">
+    <row r="176" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B176" s="16" t="s">
         <v>54</v>
       </c>
@@ -2385,14 +2401,14 @@
         <v>56</v>
       </c>
     </row>
-    <row r="177" spans="2:5">
-      <c r="B177" s="41" t="s">
+    <row r="177" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B177" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C177" s="42"/>
-      <c r="D177" s="43"/>
-    </row>
-    <row r="178" spans="2:5">
+      <c r="C177" s="41"/>
+      <c r="D177" s="42"/>
+    </row>
+    <row r="178" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B178" s="6" t="s">
         <v>3</v>
       </c>
@@ -2406,7 +2422,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="179" spans="2:5">
+    <row r="179" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B179" s="9" t="s">
         <v>33</v>
       </c>
@@ -2416,7 +2432,7 @@
       <c r="D179" s="18"/>
       <c r="E179" s="18"/>
     </row>
-    <row r="180" spans="2:5">
+    <row r="180" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B180" s="9" t="s">
         <v>34</v>
       </c>
@@ -2426,7 +2442,7 @@
       <c r="D180" s="18"/>
       <c r="E180" s="18"/>
     </row>
-    <row r="181" spans="2:5">
+    <row r="181" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B181" s="16" t="s">
         <v>28</v>
       </c>
@@ -2434,7 +2450,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="2:5">
+    <row r="182" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B182" s="16" t="s">
         <v>29</v>
       </c>
@@ -2442,7 +2458,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="184" spans="2:5" ht="14.25">
+    <row r="184" spans="2:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B184" s="37" t="s">
         <v>6</v>
       </c>
@@ -2456,7 +2472,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="185" spans="2:5">
+    <row r="185" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B185" s="14" t="s">
         <v>63</v>
       </c>
@@ -2465,15 +2481,15 @@
       </c>
       <c r="D185" s="14"/>
     </row>
-    <row r="186" spans="2:5">
-      <c r="B186" s="41" t="s">
+    <row r="186" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B186" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="C186" s="42"/>
-      <c r="D186" s="42"/>
-      <c r="E186" s="43"/>
-    </row>
-    <row r="187" spans="2:5">
+      <c r="C186" s="41"/>
+      <c r="D186" s="41"/>
+      <c r="E186" s="42"/>
+    </row>
+    <row r="187" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B187" s="15"/>
       <c r="C187" s="6" t="s">
         <v>12</v>
@@ -2485,7 +2501,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="188" spans="2:5">
+    <row r="188" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B188" s="16" t="s">
         <v>15</v>
       </c>
@@ -2497,7 +2513,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="189" spans="2:5">
+    <row r="189" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B189" s="16" t="s">
         <v>18</v>
       </c>
@@ -2505,7 +2521,7 @@
       <c r="D189" s="9"/>
       <c r="E189" s="9"/>
     </row>
-    <row r="190" spans="2:5">
+    <row r="190" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B190" s="16" t="s">
         <v>19</v>
       </c>
@@ -2515,7 +2531,7 @@
       </c>
       <c r="E190" s="9"/>
     </row>
-    <row r="191" spans="2:5">
+    <row r="191" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B191" s="16" t="s">
         <v>21</v>
       </c>
@@ -2525,7 +2541,7 @@
       </c>
       <c r="E191" s="9"/>
     </row>
-    <row r="192" spans="2:5">
+    <row r="192" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B192" s="16" t="s">
         <v>22</v>
       </c>
@@ -2535,7 +2551,7 @@
       <c r="D192" s="9"/>
       <c r="E192" s="9"/>
     </row>
-    <row r="193" spans="2:5">
+    <row r="193" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B193" s="16" t="s">
         <v>23</v>
       </c>
@@ -2543,7 +2559,7 @@
       <c r="D193" s="9"/>
       <c r="E193" s="9"/>
     </row>
-    <row r="194" spans="2:5">
+    <row r="194" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B194" s="16" t="s">
         <v>24</v>
       </c>
@@ -2551,7 +2567,7 @@
       <c r="D194" s="9"/>
       <c r="E194" s="9"/>
     </row>
-    <row r="195" spans="2:5">
+    <row r="195" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B195" s="16" t="s">
         <v>54</v>
       </c>
@@ -2559,14 +2575,14 @@
         <v>55</v>
       </c>
     </row>
-    <row r="196" spans="2:5">
-      <c r="B196" s="40" t="s">
+    <row r="196" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B196" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="C196" s="40"/>
-      <c r="D196" s="40"/>
-    </row>
-    <row r="197" spans="2:5">
+      <c r="C196" s="43"/>
+      <c r="D196" s="43"/>
+    </row>
+    <row r="197" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B197" s="6" t="s">
         <v>3</v>
       </c>
@@ -2580,7 +2596,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="198" spans="2:5">
+    <row r="198" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B198" s="9" t="s">
         <v>34</v>
       </c>
@@ -2590,7 +2606,7 @@
       <c r="D198" s="9"/>
       <c r="E198" s="9"/>
     </row>
-    <row r="199" spans="2:5">
+    <row r="199" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B199" s="9" t="s">
         <v>33</v>
       </c>
@@ -2600,7 +2616,7 @@
       <c r="D199" s="9"/>
       <c r="E199" s="9"/>
     </row>
-    <row r="200" spans="2:5">
+    <row r="200" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B200" s="16" t="s">
         <v>28</v>
       </c>
@@ -2608,7 +2624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="201" spans="2:5">
+    <row r="201" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B201" s="16" t="s">
         <v>29</v>
       </c>
@@ -2616,7 +2632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="203" spans="2:5" ht="14.25">
+    <row r="203" spans="2:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B203" s="37" t="s">
         <v>6</v>
       </c>
@@ -2628,7 +2644,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="204" spans="2:5">
+    <row r="204" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B204" s="14" t="s">
         <v>58</v>
       </c>
@@ -2636,15 +2652,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="205" spans="2:5">
-      <c r="B205" s="40" t="s">
+    <row r="205" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B205" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C205" s="40"/>
-      <c r="D205" s="40"/>
-      <c r="E205" s="40"/>
-    </row>
-    <row r="206" spans="2:5">
+      <c r="C205" s="43"/>
+      <c r="D205" s="43"/>
+      <c r="E205" s="43"/>
+    </row>
+    <row r="206" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B206" s="15"/>
       <c r="C206" s="6" t="s">
         <v>12</v>
@@ -2656,7 +2672,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="207" spans="2:5">
+    <row r="207" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B207" s="16" t="s">
         <v>15</v>
       </c>
@@ -2668,7 +2684,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="208" spans="2:5">
+    <row r="208" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B208" s="16" t="s">
         <v>18</v>
       </c>
@@ -2676,7 +2692,7 @@
       <c r="D208" s="9"/>
       <c r="E208" s="9"/>
     </row>
-    <row r="209" spans="2:5">
+    <row r="209" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B209" s="16" t="s">
         <v>19</v>
       </c>
@@ -2686,7 +2702,7 @@
       </c>
       <c r="E209" s="9"/>
     </row>
-    <row r="210" spans="2:5">
+    <row r="210" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B210" s="16" t="s">
         <v>21</v>
       </c>
@@ -2696,7 +2712,7 @@
       </c>
       <c r="E210" s="9"/>
     </row>
-    <row r="211" spans="2:5">
+    <row r="211" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B211" s="16" t="s">
         <v>22</v>
       </c>
@@ -2706,7 +2722,7 @@
       <c r="D211" s="9"/>
       <c r="E211" s="9"/>
     </row>
-    <row r="212" spans="2:5">
+    <row r="212" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B212" s="16" t="s">
         <v>23</v>
       </c>
@@ -2714,7 +2730,7 @@
       <c r="D212" s="9"/>
       <c r="E212" s="9"/>
     </row>
-    <row r="213" spans="2:5">
+    <row r="213" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B213" s="16" t="s">
         <v>24</v>
       </c>
@@ -2722,7 +2738,7 @@
       <c r="D213" s="9"/>
       <c r="E213" s="9"/>
     </row>
-    <row r="214" spans="2:5">
+    <row r="214" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B214" s="16" t="s">
         <v>54</v>
       </c>
@@ -2730,14 +2746,14 @@
         <v>56</v>
       </c>
     </row>
-    <row r="215" spans="2:5">
-      <c r="B215" s="40" t="s">
+    <row r="215" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B215" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="C215" s="40"/>
-      <c r="D215" s="40"/>
-    </row>
-    <row r="216" spans="2:5">
+      <c r="C215" s="43"/>
+      <c r="D215" s="43"/>
+    </row>
+    <row r="216" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B216" s="6" t="s">
         <v>3</v>
       </c>
@@ -2751,7 +2767,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="217" spans="2:5">
+    <row r="217" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B217" s="9" t="s">
         <v>33</v>
       </c>
@@ -2761,7 +2777,7 @@
       <c r="D217" s="9"/>
       <c r="E217" s="18"/>
     </row>
-    <row r="218" spans="2:5">
+    <row r="218" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B218" s="9" t="s">
         <v>34</v>
       </c>
@@ -2771,7 +2787,7 @@
       <c r="D218" s="9"/>
       <c r="E218" s="9"/>
     </row>
-    <row r="219" spans="2:5">
+    <row r="219" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B219" s="16" t="s">
         <v>28</v>
       </c>
@@ -2779,7 +2795,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="220" spans="2:5">
+    <row r="220" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B220" s="16" t="s">
         <v>29</v>
       </c>
@@ -2787,7 +2803,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="222" spans="2:5" ht="14.25">
+    <row r="222" spans="2:5" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B222" s="37" t="s">
         <v>6</v>
       </c>
@@ -2801,7 +2817,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="223" spans="2:5">
+    <row r="223" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B223" s="14" t="s">
         <v>65</v>
       </c>
@@ -2810,15 +2826,15 @@
       </c>
       <c r="D223" s="14"/>
     </row>
-    <row r="224" spans="2:5">
-      <c r="B224" s="41" t="s">
+    <row r="224" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B224" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="C224" s="42"/>
-      <c r="D224" s="42"/>
-      <c r="E224" s="43"/>
-    </row>
-    <row r="225" spans="2:5">
+      <c r="C224" s="41"/>
+      <c r="D224" s="41"/>
+      <c r="E224" s="42"/>
+    </row>
+    <row r="225" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B225" s="15"/>
       <c r="C225" s="6" t="s">
         <v>12</v>
@@ -2830,7 +2846,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="226" spans="2:5">
+    <row r="226" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B226" s="16" t="s">
         <v>15</v>
       </c>
@@ -2842,7 +2858,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="227" spans="2:5">
+    <row r="227" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B227" s="16" t="s">
         <v>18</v>
       </c>
@@ -2850,7 +2866,7 @@
       <c r="D227" s="9"/>
       <c r="E227" s="9"/>
     </row>
-    <row r="228" spans="2:5">
+    <row r="228" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B228" s="16" t="s">
         <v>19</v>
       </c>
@@ -2860,7 +2876,7 @@
       </c>
       <c r="E228" s="9"/>
     </row>
-    <row r="229" spans="2:5">
+    <row r="229" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B229" s="16" t="s">
         <v>21</v>
       </c>
@@ -2870,7 +2886,7 @@
       </c>
       <c r="E229" s="9"/>
     </row>
-    <row r="230" spans="2:5">
+    <row r="230" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B230" s="16" t="s">
         <v>22</v>
       </c>
@@ -2880,7 +2896,7 @@
       <c r="D230" s="9"/>
       <c r="E230" s="9"/>
     </row>
-    <row r="231" spans="2:5">
+    <row r="231" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B231" s="16" t="s">
         <v>23</v>
       </c>
@@ -2888,7 +2904,7 @@
       <c r="D231" s="9"/>
       <c r="E231" s="9"/>
     </row>
-    <row r="232" spans="2:5">
+    <row r="232" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B232" s="16" t="s">
         <v>24</v>
       </c>
@@ -2898,7 +2914,7 @@
       </c>
       <c r="E232" s="9"/>
     </row>
-    <row r="233" spans="2:5">
+    <row r="233" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B233" s="16" t="s">
         <v>54</v>
       </c>
@@ -2906,14 +2922,14 @@
         <v>56</v>
       </c>
     </row>
-    <row r="234" spans="2:5">
-      <c r="B234" s="41" t="s">
+    <row r="234" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B234" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C234" s="42"/>
-      <c r="D234" s="43"/>
-    </row>
-    <row r="235" spans="2:5">
+      <c r="C234" s="41"/>
+      <c r="D234" s="42"/>
+    </row>
+    <row r="235" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B235" s="6" t="s">
         <v>3</v>
       </c>
@@ -2927,7 +2943,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="236" spans="2:5">
+    <row r="236" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B236" s="9" t="s">
         <v>33</v>
       </c>
@@ -2937,7 +2953,7 @@
       <c r="D236" s="18"/>
       <c r="E236" s="18"/>
     </row>
-    <row r="237" spans="2:5">
+    <row r="237" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B237" s="9" t="s">
         <v>34</v>
       </c>
@@ -2947,7 +2963,7 @@
       <c r="D237" s="18"/>
       <c r="E237" s="18"/>
     </row>
-    <row r="238" spans="2:5">
+    <row r="238" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B238" s="16" t="s">
         <v>28</v>
       </c>
@@ -2955,7 +2971,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="239" spans="2:5">
+    <row r="239" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B239" s="16" t="s">
         <v>29</v>
       </c>
@@ -2966,20 +2982,14 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="31">
-    <mergeCell ref="B105:E105"/>
-    <mergeCell ref="B115:D115"/>
-    <mergeCell ref="B132:D132"/>
-    <mergeCell ref="B124:D124"/>
-    <mergeCell ref="B126:D126"/>
-    <mergeCell ref="B127:C127"/>
-    <mergeCell ref="B128:C128"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B96:D96"/>
-    <mergeCell ref="B86:E86"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="B77:D77"/>
+    <mergeCell ref="B215:D215"/>
+    <mergeCell ref="B224:E224"/>
+    <mergeCell ref="B234:D234"/>
+    <mergeCell ref="B167:E167"/>
+    <mergeCell ref="B177:D177"/>
+    <mergeCell ref="B186:E186"/>
+    <mergeCell ref="B196:D196"/>
+    <mergeCell ref="B205:E205"/>
     <mergeCell ref="B134:D134"/>
     <mergeCell ref="B135:C135"/>
     <mergeCell ref="B136:C136"/>
@@ -2989,14 +2999,20 @@
     <mergeCell ref="B142:D142"/>
     <mergeCell ref="B143:C143"/>
     <mergeCell ref="B144:C144"/>
-    <mergeCell ref="B215:D215"/>
-    <mergeCell ref="B224:E224"/>
-    <mergeCell ref="B234:D234"/>
-    <mergeCell ref="B167:E167"/>
-    <mergeCell ref="B177:D177"/>
-    <mergeCell ref="B186:E186"/>
-    <mergeCell ref="B196:D196"/>
-    <mergeCell ref="B205:E205"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B96:D96"/>
+    <mergeCell ref="B86:E86"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="B77:D77"/>
+    <mergeCell ref="B105:E105"/>
+    <mergeCell ref="B115:D115"/>
+    <mergeCell ref="B132:D132"/>
+    <mergeCell ref="B124:D124"/>
+    <mergeCell ref="B126:D126"/>
+    <mergeCell ref="B127:C127"/>
+    <mergeCell ref="B128:C128"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3019,44 +3035,44 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.5703125" style="26" customWidth="1"/>
     <col min="2" max="2" width="134.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1" s="19" t="str">
         <f>"&lt;forecast seriesName="&amp;CHAR(34)&amp;Schedules!D2&amp;CHAR(34)&amp;"&gt;"</f>
         <v>&lt;forecast seriesName="MeningococcalB"&gt;</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2" s="19" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B4&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C4&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Bexsero" vaccineIds="216"/&gt;</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B3" s="19" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B5&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C5&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Trumenba" vaccineIds="215"/&gt;</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B4" s="19" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B6&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C6&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Men B" vaccineIds="215, 216"/&gt;</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
         <v>41</v>
       </c>
@@ -3065,73 +3081,73 @@
         <v xml:space="preserve">  &lt;schedule scheduleName="P1" dose="1" indication="DOSERECEIVED" label="1st"&gt;</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B6" s="19" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C63&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C62&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="1"/&gt;</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B7" s="20" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C51&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D51&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E51&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;valid age="16 years" interval="" grace="4 days"/&gt;</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v xml:space="preserve">    &lt;valid age="10 years" interval="" grace="4 days"/&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B8" s="20" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C52&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D52&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E52&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B9" s="20" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C53&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D53&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E53&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="16 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B10" s="20" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C54&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D54&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E54&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="19 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B11" s="20" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C55&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D55&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E55&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="24 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B12" s="20" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D56&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E56&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="0 days" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B13" s="20" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D57&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B14" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B60&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C60&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D60&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E60&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Bexsero" schedule="B2" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B15" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B61&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C61&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D61&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E61&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Trumenba" schedule="T2" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B16" s="20" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="27" t="s">
         <v>39</v>
       </c>
@@ -3140,79 +3156,79 @@
         <v xml:space="preserve">  &lt;schedule scheduleName="T2" dose="2" indication="" label="2nd"&gt;</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B18" s="19" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C82&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C81&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="2" column="2"/&gt;</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B19" s="20" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C69&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D69&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E69&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="" interval="6 months" grace="6 months"/&gt;</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B20" s="20" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C70&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D70&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E70&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B21" s="20" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C71&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D71&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E71&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="" interval="6 months" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B22" s="20" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C72&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D72&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E72&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="" interval="7 months" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B23" s="20" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C73&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D73&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E73&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="24 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B24" s="20" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D74&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E74&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B25" s="20" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D75&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B26" s="20" t="str">
         <f>"    &lt;recommend seriesName="&amp;CHAR(34)&amp;Schedules!C76&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;recommend seriesName="MeningTrumenba"/&gt;</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B27" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B79&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C79&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D79&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E79&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Bexsero" schedule="B2a" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B28" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B80&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C80&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D80&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E80&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Trumenba" schedule="DL Trumenba A" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B29" s="20" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="27" t="s">
         <v>43</v>
       </c>
@@ -3221,79 +3237,79 @@
         <v xml:space="preserve">  &lt;schedule scheduleName="B2" dose="2" indication="" label="2nd"&gt;</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B31" s="19" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C101&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C100&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="2"/&gt;</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B32" s="20" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C88&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D88&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E88&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="" interval="4 weeks" grace="4 weeks"/&gt;</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B33" s="20" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C89&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D89&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E89&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B34" s="20" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C90&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D90&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E90&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="" interval="4 weeks" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B35" s="20" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C91&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D91&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E91&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="" interval="2 months" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B36" s="20" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C92&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D92&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E92&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="24 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B37" s="20" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D93&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E93&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B38" s="20" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D94&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B39" s="20" t="str">
         <f>"    &lt;recommend seriesName="&amp;CHAR(34)&amp;Schedules!C95&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;recommend seriesName="MeningBexsero"/&gt;</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B40" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B98&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C98&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D98&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E98&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Trumenba" schedule="T2a" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B41" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B99&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C99&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D99&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E99&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Bexsero" schedule="COMPLETE" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B42" s="20" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="27" t="str">
         <f>Schedules!B123</f>
         <v>DL Trumenba A</v>
@@ -3303,30 +3319,30 @@
         <v xml:space="preserve">  &lt;decisionLogic name="DL Trumenba A"&gt;</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B44" s="20" t="str">
         <f>"    &lt;constant name="&amp;CHAR(34)&amp;Schedules!B125&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D125&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;constant name="Valid Vaccine" value="Trumenba"/&gt;</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B45" s="20" t="str">
         <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B127&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D127&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;transition name="Greater Than 6 Months" value="COMPLETE"/&gt;</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B46" s="20" t="str">
         <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B128&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D128&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;transition name="Less Than 6 Months" value="T3"/&gt;</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B47" s="20" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="27" t="str">
         <f>Schedules!B131</f>
         <v>DL Trumenba B</v>
@@ -3336,30 +3352,30 @@
         <v xml:space="preserve">  &lt;decisionLogic name="DL Trumenba B"&gt;</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B49" s="20" t="str">
         <f>"    &lt;constant name="&amp;CHAR(34)&amp;Schedules!B133&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D133&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;constant name="Valid Vaccine" value="Trumenba"/&gt;</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B50" s="20" t="str">
         <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B135&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D135&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;transition name="Greater Than 6 Months" value="COMPLETE"/&gt;</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B51" s="20" t="str">
         <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B136&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D136&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;transition name="Less Than 6 Months" value="T3a"/&gt;</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B52" s="20" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="27" t="str">
         <f>Schedules!B139</f>
         <v>DL Trumenba C</v>
@@ -3369,30 +3385,30 @@
         <v xml:space="preserve">  &lt;decisionLogic name="DL Trumenba C"&gt;</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B54" s="20" t="str">
         <f>"    &lt;constant name="&amp;CHAR(34)&amp;Schedules!B141&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D141&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;constant name="Valid Vaccine" value="Trumenba"/&gt;</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B55" s="20" t="str">
         <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B143&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D143&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;transition name="Greater Than 6 Months" value="COMPLETE"/&gt;</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B56" s="20" t="str">
         <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B144&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D144&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;transition name="Less Than 6 Months" value="T3b"/&gt;</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B57" s="20" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="27" t="str">
         <f>Schedules!B104</f>
         <v>T3</v>
@@ -3402,79 +3418,79 @@
         <v xml:space="preserve">  &lt;schedule scheduleName="T3" dose="3" indication="" label="3rd"&gt;</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B59" s="19" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C120&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C119&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="2" column="3"/&gt;</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B60" s="20" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C107&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D107&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E107&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="" interval="4 weeks" grace="4 weeks"/&gt;</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B61" s="20" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C108&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D108&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E108&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B62" s="20" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C109&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D109&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E109&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="" interval="4 weeks" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B63" s="20" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C110&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D110&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E110&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="" interval="2 months" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B64" s="20" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C111&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D111&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E111&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="24 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B65" s="20" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D112&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E112&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B66" s="20" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D113&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval="6 months"/&gt;</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B67" s="20" t="str">
         <f>"    &lt;recommend seriesName="&amp;CHAR(34)&amp;Schedules!C114&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;recommend seriesName="MeningTrumenba"/&gt;</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B68" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B117&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C117&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D117&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E117&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Bexsero" schedule="B2b" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B69" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B118&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C118&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D118&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E118&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Trumenba" schedule="COMPLETE" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B70" s="20" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="27" t="str">
         <f>Schedules!B147</f>
         <v>B2a</v>
@@ -3484,79 +3500,79 @@
         <v xml:space="preserve">  &lt;schedule scheduleName="B2a" dose="2" indication="" label="2nd"&gt;</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B72" s="19" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C163&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C162&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="3" column="2"/&gt;</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B73" s="20" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C150&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D150&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E150&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="" interval="4 weeks" grace="4 weeks"/&gt;</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B74" s="20" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C151&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D151&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E151&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B75" s="20" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C152&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D152&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E152&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="" interval="4 weeks" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B76" s="20" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C153&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D153&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E153&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="" interval="2 months" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B77" s="20" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C154&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D154&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E154&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="24 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B78" s="20" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D155&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E155&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B79" s="20" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D156&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B80" s="20" t="str">
         <f>"    &lt;recommend seriesName="&amp;CHAR(34)&amp;Schedules!C157&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;recommend seriesName="MeningBexsero"/&gt;</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B81" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B160&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C160&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D160&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E160&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Trumenba" schedule="DL Trumenba B" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B82" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B161&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C161&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D161&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E161&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Bexsero" schedule="COMPLETE" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B83" s="20" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="27" t="str">
         <f>Schedules!B166</f>
         <v>T3a</v>
@@ -3566,79 +3582,79 @@
         <v xml:space="preserve">  &lt;schedule scheduleName="T3a" dose="3" indication="" label="3rd"&gt;</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B85" s="19" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C182&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C181&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="3" column="3"/&gt;</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B86" s="20" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C169&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D169&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E169&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="" interval="4 weeks" grace="4 weeks"/&gt;</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B87" s="20" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C170&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D170&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E170&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B88" s="20" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C171&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D171&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E171&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="" interval="4 weeks" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B89" s="20" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C172&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D172&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E172&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="" interval="2 months" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B90" s="20" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C173&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D173&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E173&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="24 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B91" s="20" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D174&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E174&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B92" s="20" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D175&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval="6 months"/&gt;</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B93" s="20" t="str">
         <f>"    &lt;recommend seriesName="&amp;CHAR(34)&amp;Schedules!C176&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;recommend seriesName="MeningTrumenba"/&gt;</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B94" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B179&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C179&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D179&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E179&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Bexsero" schedule="COMPLETE" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B95" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B180&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C180&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D180&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E180&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Trumenba" schedule="COMPLETE" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B96" s="20" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="27" t="str">
         <f>Schedules!B185</f>
         <v>B2b</v>
@@ -3648,79 +3664,79 @@
         <v xml:space="preserve">  &lt;schedule scheduleName="B2b" dose="2" indication="" label="2nd"&gt;</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B98" s="19" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C201&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C200&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="2" column="4"/&gt;</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B99" s="20" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C188&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D188&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E188&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="" interval="4 weeks" grace="4 weeks"/&gt;</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B100" s="20" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C189&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D189&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E189&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B101" s="20" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C190&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D190&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E190&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="" interval="4 weeks" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B102" s="20" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C191&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D191&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E191&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="" interval="2 months" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B103" s="20" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C192&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D192&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E192&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="24 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B104" s="20" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D193&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E193&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B105" s="20" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D194&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B106" s="20" t="str">
         <f>"    &lt;recommend seriesName="&amp;CHAR(34)&amp;Schedules!C195&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;recommend seriesName="MeningBexsero"/&gt;</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B107" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B198&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C198&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D198&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E198&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Trumenba" schedule="COMPLETE" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B108" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B199&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C199&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D199&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E199&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Bexsero" schedule="COMPLETE" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B109" s="20" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="27" t="str">
         <f>Schedules!B204</f>
         <v>T2a</v>
@@ -3730,79 +3746,79 @@
         <v xml:space="preserve">  &lt;schedule scheduleName="T2a" dose="2" indication="" label="2nd"&gt;</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B111" s="19" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C220&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C219&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="2" column="2"/&gt;</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B112" s="20" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C207&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D207&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E207&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="" interval="6 months" grace="6 months"/&gt;</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B113" s="20" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C208&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D208&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E208&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B114" s="20" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C209&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D209&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E209&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="" interval="6 months" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B115" s="20" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C210&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D210&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E210&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="" interval="7 months" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B116" s="20" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C211&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D211&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E211&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="24 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B117" s="20" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D212&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E212&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B118" s="20" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D213&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B119" s="20" t="str">
         <f>"    &lt;recommend seriesName="&amp;CHAR(34)&amp;Schedules!C214&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;recommend seriesName="MeningTrumenba"/&gt;</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B120" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B217&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C217&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D217&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E217&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Bexsero" schedule="COMPLETE" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B121" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B218&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C218&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D218&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E218&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Trumenba" schedule="DL Trumenba C" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B122" s="20" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="27" t="str">
         <f>Schedules!B223</f>
         <v>T3b</v>
@@ -3812,79 +3828,79 @@
         <v xml:space="preserve">  &lt;schedule scheduleName="T3b" dose="3" indication="" label="3rd"&gt;</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B124" s="19" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C239&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C238&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="3" column="3"/&gt;</v>
       </c>
     </row>
-    <row r="125" spans="1:2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B125" s="20" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C226&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D226&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E226&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="" interval="4 weeks" grace="4 weeks"/&gt;</v>
       </c>
     </row>
-    <row r="126" spans="1:2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B126" s="20" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C227&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D227&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E227&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B127" s="20" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C228&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D228&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E228&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="" interval="4 weeks" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B128" s="20" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C229&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D229&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E229&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="" interval="2 months" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="129" spans="2:2">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B129" s="20" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C230&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D230&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E230&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="24 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="130" spans="2:2">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B130" s="20" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D231&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E231&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="131" spans="2:2">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B131" s="20" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D232&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval="6 months"/&gt;</v>
       </c>
     </row>
-    <row r="132" spans="2:2">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B132" s="20" t="str">
         <f>"    &lt;recommend seriesName="&amp;CHAR(34)&amp;Schedules!C233&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;recommend seriesName="MeningTrumenba"/&gt;</v>
       </c>
     </row>
-    <row r="133" spans="2:2">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B133" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B236&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C236&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D236&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E236&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Bexsero" schedule="COMPLETE" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="134" spans="2:2">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B134" s="20" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B237&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C237&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D237&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E237&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Trumenba" schedule="COMPLETE" age="" reason=""/&gt;</v>
       </c>
     </row>
-    <row r="135" spans="2:2">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B135" s="20" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="136" spans="2:2">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B136" s="30" t="str">
         <f>"&lt;/forecast&gt;"</f>
         <v>&lt;/forecast&gt;</v>

</xml_diff>

<commit_message>
Three changes: (1) Men B indication changed to birth (2) MCV4 finished age 22 (previously 19 years) (3) Flu de-duplication issue fixed. Change the version number 4.2.0
</commit_message>
<xml_diff>
--- a/schedules/MeningococcalB.xlsx
+++ b/schedules/MeningococcalB.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\IMMUN\Claire\Forecaster\Mening B\12.28.17 forecaster document copies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\IMMUN\Forecaster\Schedules &amp; Tables\Schedule Development\Knowledge Transfer\MenB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18285" windowHeight="9675" tabRatio="242"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22575" windowHeight="10860" tabRatio="242"/>
   </bookViews>
   <sheets>
     <sheet name="Schedules" sheetId="1" r:id="rId1"/>
@@ -186,9 +186,6 @@
     <t>24 years</t>
   </si>
   <si>
-    <t>DOSERECEIVED</t>
-  </si>
-  <si>
     <t>19 years</t>
   </si>
   <si>
@@ -275,6 +272,9 @@
   </si>
   <si>
     <t>10 years</t>
+  </si>
+  <si>
+    <t>BIRTH</t>
   </si>
 </sst>
 </file>
@@ -599,6 +599,9 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -606,9 +609,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -706,40 +706,39 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>104774</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9527</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>116365</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>200024</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>809625</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>146125</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:srcRect r="3818"/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="104774" y="1076325"/>
-          <a:ext cx="7553325" cy="6137350"/>
+          <a:off x="114302" y="1030765"/>
+          <a:ext cx="7200898" cy="6084410"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1101,8 +1100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I239"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J54" sqref="J54"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1122,18 +1121,18 @@
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>2</v>
@@ -1285,16 +1284,16 @@
         <v>1</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B49" s="40" t="s">
+      <c r="B49" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="C49" s="41"/>
-      <c r="D49" s="41"/>
-      <c r="E49" s="42"/>
+      <c r="C49" s="42"/>
+      <c r="D49" s="42"/>
+      <c r="E49" s="43"/>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B50" s="15"/>
@@ -1313,7 +1312,7 @@
         <v>15</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D51" s="9"/>
       <c r="E51" s="9" t="s">
@@ -1343,7 +1342,7 @@
         <v>21</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
@@ -1377,11 +1376,11 @@
       <c r="E57" s="9"/>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B58" s="43" t="s">
+      <c r="B58" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C58" s="43"/>
-      <c r="D58" s="43"/>
+      <c r="C58" s="40"/>
+      <c r="D58" s="40"/>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B59" s="6" t="s">
@@ -1454,12 +1453,12 @@
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B67" s="43" t="s">
+      <c r="B67" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="C67" s="43"/>
-      <c r="D67" s="43"/>
-      <c r="E67" s="43"/>
+      <c r="C67" s="40"/>
+      <c r="D67" s="40"/>
+      <c r="E67" s="40"/>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B68" s="15"/>
@@ -1509,7 +1508,7 @@
       </c>
       <c r="C72" s="9"/>
       <c r="D72" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E72" s="9"/>
     </row>
@@ -1541,18 +1540,18 @@
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B76" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B77" s="43" t="s">
+      <c r="B77" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C77" s="43"/>
-      <c r="D77" s="43"/>
+      <c r="C77" s="40"/>
+      <c r="D77" s="40"/>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B78" s="6" t="s">
@@ -1573,7 +1572,7 @@
         <v>33</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D79" s="9"/>
       <c r="E79" s="18"/>
@@ -1583,7 +1582,7 @@
         <v>34</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D80" s="9"/>
       <c r="E80" s="9"/>
@@ -1628,12 +1627,12 @@
       <c r="D85" s="14"/>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B86" s="40" t="s">
+      <c r="B86" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="C86" s="41"/>
-      <c r="D86" s="41"/>
-      <c r="E86" s="42"/>
+      <c r="C86" s="42"/>
+      <c r="D86" s="42"/>
+      <c r="E86" s="43"/>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B87" s="15"/>
@@ -1715,18 +1714,18 @@
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B95" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C95" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C95" s="9" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B96" s="43" t="s">
+      <c r="B96" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C96" s="43"/>
-      <c r="D96" s="43"/>
+      <c r="C96" s="40"/>
+      <c r="D96" s="40"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B97" s="6" t="s">
@@ -1747,7 +1746,7 @@
         <v>34</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D98" s="9"/>
       <c r="E98" s="18"/>
@@ -1790,12 +1789,12 @@
         <v>8</v>
       </c>
       <c r="E103" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B104" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C104" s="14">
         <v>3</v>
@@ -1803,12 +1802,12 @@
       <c r="D104" s="14"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B105" s="40" t="s">
+      <c r="B105" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="C105" s="41"/>
-      <c r="D105" s="41"/>
-      <c r="E105" s="42"/>
+      <c r="C105" s="42"/>
+      <c r="D105" s="42"/>
+      <c r="E105" s="43"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B106" s="15"/>
@@ -1892,18 +1891,18 @@
     </row>
     <row r="114" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B114" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C114" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="115" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B115" s="40" t="s">
+      <c r="B115" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="C115" s="41"/>
-      <c r="D115" s="42"/>
+      <c r="C115" s="42"/>
+      <c r="D115" s="43"/>
     </row>
     <row r="116" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B116" s="6" t="s">
@@ -1924,7 +1923,7 @@
         <v>33</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D117" s="18"/>
       <c r="E117" s="18"/>
@@ -1957,24 +1956,24 @@
     </row>
     <row r="122" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B122" s="32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="123" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B123" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="124" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B124" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="C124" s="43"/>
-      <c r="D124" s="43"/>
+      <c r="B124" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="C124" s="40"/>
+      <c r="D124" s="40"/>
     </row>
     <row r="125" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B125" s="35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C125" s="36"/>
       <c r="D125" s="25" t="s">
@@ -1982,15 +1981,15 @@
       </c>
     </row>
     <row r="126" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B126" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="C126" s="43"/>
-      <c r="D126" s="43"/>
+      <c r="B126" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="C126" s="40"/>
+      <c r="D126" s="40"/>
     </row>
     <row r="127" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B127" s="44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C127" s="45"/>
       <c r="D127" s="29" t="s">
@@ -1999,33 +1998,33 @@
     </row>
     <row r="128" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B128" s="44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C128" s="45"/>
       <c r="D128" s="29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="130" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B130" s="32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="131" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B131" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="132" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B132" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="C132" s="43"/>
-      <c r="D132" s="43"/>
+      <c r="B132" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="C132" s="40"/>
+      <c r="D132" s="40"/>
     </row>
     <row r="133" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B133" s="33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C133" s="34"/>
       <c r="D133" s="25" t="s">
@@ -2033,15 +2032,15 @@
       </c>
     </row>
     <row r="134" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B134" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="C134" s="43"/>
-      <c r="D134" s="43"/>
+      <c r="B134" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="C134" s="40"/>
+      <c r="D134" s="40"/>
     </row>
     <row r="135" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B135" s="44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C135" s="45"/>
       <c r="D135" s="29" t="s">
@@ -2050,33 +2049,33 @@
     </row>
     <row r="136" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B136" s="44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C136" s="45"/>
       <c r="D136" s="29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="138" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B138" s="37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="139" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B139" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="140" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B140" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="C140" s="43"/>
-      <c r="D140" s="43"/>
+      <c r="B140" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="C140" s="40"/>
+      <c r="D140" s="40"/>
     </row>
     <row r="141" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B141" s="38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C141" s="39"/>
       <c r="D141" s="25" t="s">
@@ -2084,15 +2083,15 @@
       </c>
     </row>
     <row r="142" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B142" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="C142" s="43"/>
-      <c r="D142" s="43"/>
+      <c r="B142" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="C142" s="40"/>
+      <c r="D142" s="40"/>
     </row>
     <row r="143" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B143" s="44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C143" s="45"/>
       <c r="D143" s="29" t="s">
@@ -2101,11 +2100,11 @@
     </row>
     <row r="144" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B144" s="44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C144" s="45"/>
       <c r="D144" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="146" spans="2:5" ht="14.25" x14ac:dyDescent="0.2">
@@ -2124,7 +2123,7 @@
     </row>
     <row r="147" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B147" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C147" s="14">
         <v>2</v>
@@ -2132,12 +2131,12 @@
       <c r="D147" s="14"/>
     </row>
     <row r="148" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B148" s="40" t="s">
+      <c r="B148" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="C148" s="41"/>
-      <c r="D148" s="41"/>
-      <c r="E148" s="42"/>
+      <c r="C148" s="42"/>
+      <c r="D148" s="42"/>
+      <c r="E148" s="43"/>
     </row>
     <row r="149" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B149" s="15"/>
@@ -2219,18 +2218,18 @@
     </row>
     <row r="157" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B157" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C157" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C157" s="9" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="158" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B158" s="43" t="s">
+      <c r="B158" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C158" s="43"/>
-      <c r="D158" s="43"/>
+      <c r="C158" s="40"/>
+      <c r="D158" s="40"/>
     </row>
     <row r="159" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B159" s="6" t="s">
@@ -2251,7 +2250,7 @@
         <v>34</v>
       </c>
       <c r="C160" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D160" s="9"/>
       <c r="E160" s="9"/>
@@ -2293,12 +2292,12 @@
         <v>8</v>
       </c>
       <c r="E165" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="166" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B166" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C166" s="14">
         <v>3</v>
@@ -2306,12 +2305,12 @@
       <c r="D166" s="14"/>
     </row>
     <row r="167" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B167" s="40" t="s">
+      <c r="B167" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="C167" s="41"/>
-      <c r="D167" s="41"/>
-      <c r="E167" s="42"/>
+      <c r="C167" s="42"/>
+      <c r="D167" s="42"/>
+      <c r="E167" s="43"/>
     </row>
     <row r="168" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B168" s="15"/>
@@ -2395,18 +2394,18 @@
     </row>
     <row r="176" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B176" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C176" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="177" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B177" s="40" t="s">
+      <c r="B177" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="C177" s="41"/>
-      <c r="D177" s="42"/>
+      <c r="C177" s="42"/>
+      <c r="D177" s="43"/>
     </row>
     <row r="178" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B178" s="6" t="s">
@@ -2474,7 +2473,7 @@
     </row>
     <row r="185" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B185" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C185" s="14">
         <v>2</v>
@@ -2482,12 +2481,12 @@
       <c r="D185" s="14"/>
     </row>
     <row r="186" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B186" s="40" t="s">
+      <c r="B186" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="C186" s="41"/>
-      <c r="D186" s="41"/>
-      <c r="E186" s="42"/>
+      <c r="C186" s="42"/>
+      <c r="D186" s="42"/>
+      <c r="E186" s="43"/>
     </row>
     <row r="187" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B187" s="15"/>
@@ -2569,18 +2568,18 @@
     </row>
     <row r="195" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B195" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C195" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C195" s="9" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="196" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B196" s="43" t="s">
+      <c r="B196" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C196" s="43"/>
-      <c r="D196" s="43"/>
+      <c r="C196" s="40"/>
+      <c r="D196" s="40"/>
     </row>
     <row r="197" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B197" s="6" t="s">
@@ -2646,19 +2645,19 @@
     </row>
     <row r="204" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B204" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C204" s="14">
         <v>2</v>
       </c>
     </row>
     <row r="205" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B205" s="43" t="s">
+      <c r="B205" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="C205" s="43"/>
-      <c r="D205" s="43"/>
-      <c r="E205" s="43"/>
+      <c r="C205" s="40"/>
+      <c r="D205" s="40"/>
+      <c r="E205" s="40"/>
     </row>
     <row r="206" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B206" s="15"/>
@@ -2708,7 +2707,7 @@
       </c>
       <c r="C210" s="9"/>
       <c r="D210" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E210" s="9"/>
     </row>
@@ -2740,18 +2739,18 @@
     </row>
     <row r="214" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B214" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C214" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="215" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B215" s="43" t="s">
+      <c r="B215" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C215" s="43"/>
-      <c r="D215" s="43"/>
+      <c r="C215" s="40"/>
+      <c r="D215" s="40"/>
     </row>
     <row r="216" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B216" s="6" t="s">
@@ -2782,7 +2781,7 @@
         <v>34</v>
       </c>
       <c r="C218" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D218" s="9"/>
       <c r="E218" s="9"/>
@@ -2814,12 +2813,12 @@
         <v>8</v>
       </c>
       <c r="E222" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="223" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B223" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C223" s="14">
         <v>3</v>
@@ -2827,12 +2826,12 @@
       <c r="D223" s="14"/>
     </row>
     <row r="224" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B224" s="40" t="s">
+      <c r="B224" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="C224" s="41"/>
-      <c r="D224" s="41"/>
-      <c r="E224" s="42"/>
+      <c r="C224" s="42"/>
+      <c r="D224" s="42"/>
+      <c r="E224" s="43"/>
     </row>
     <row r="225" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B225" s="15"/>
@@ -2916,18 +2915,18 @@
     </row>
     <row r="233" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B233" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C233" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="234" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B234" s="40" t="s">
+      <c r="B234" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="C234" s="41"/>
-      <c r="D234" s="42"/>
+      <c r="C234" s="42"/>
+      <c r="D234" s="43"/>
     </row>
     <row r="235" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B235" s="6" t="s">
@@ -2982,14 +2981,20 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="31">
-    <mergeCell ref="B215:D215"/>
-    <mergeCell ref="B224:E224"/>
-    <mergeCell ref="B234:D234"/>
-    <mergeCell ref="B167:E167"/>
-    <mergeCell ref="B177:D177"/>
-    <mergeCell ref="B186:E186"/>
-    <mergeCell ref="B196:D196"/>
-    <mergeCell ref="B205:E205"/>
+    <mergeCell ref="B105:E105"/>
+    <mergeCell ref="B115:D115"/>
+    <mergeCell ref="B132:D132"/>
+    <mergeCell ref="B124:D124"/>
+    <mergeCell ref="B126:D126"/>
+    <mergeCell ref="B127:C127"/>
+    <mergeCell ref="B128:C128"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B96:D96"/>
+    <mergeCell ref="B86:E86"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="B77:D77"/>
     <mergeCell ref="B134:D134"/>
     <mergeCell ref="B135:C135"/>
     <mergeCell ref="B136:C136"/>
@@ -2999,27 +3004,21 @@
     <mergeCell ref="B142:D142"/>
     <mergeCell ref="B143:C143"/>
     <mergeCell ref="B144:C144"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B96:D96"/>
-    <mergeCell ref="B86:E86"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="B77:D77"/>
-    <mergeCell ref="B105:E105"/>
-    <mergeCell ref="B115:D115"/>
-    <mergeCell ref="B132:D132"/>
-    <mergeCell ref="B124:D124"/>
-    <mergeCell ref="B126:D126"/>
-    <mergeCell ref="B127:C127"/>
-    <mergeCell ref="B128:C128"/>
+    <mergeCell ref="B215:D215"/>
+    <mergeCell ref="B224:E224"/>
+    <mergeCell ref="B234:D234"/>
+    <mergeCell ref="B167:E167"/>
+    <mergeCell ref="B177:D177"/>
+    <mergeCell ref="B186:E186"/>
+    <mergeCell ref="B196:D196"/>
+    <mergeCell ref="B205:E205"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;F</oddHeader>
-    <oddFooter>Prepared by Brady Kerr &amp;D&amp;RPage &amp;P</oddFooter>
+    <oddFooter>&amp;CRevised by Claire Cook &amp;D&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <rowBreaks count="7" manualBreakCount="7">
     <brk id="7" max="8" man="1"/>
@@ -3038,8 +3037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B136"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3078,7 +3077,7 @@
       </c>
       <c r="B5" s="20" t="str">
         <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B48&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C48&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D48&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E47&amp;CHAR(34)&amp;"&gt;"</f>
-        <v xml:space="preserve">  &lt;schedule scheduleName="P1" dose="1" indication="DOSERECEIVED" label="1st"&gt;</v>
+        <v xml:space="preserve">  &lt;schedule scheduleName="P1" dose="1" indication="BIRTH" label="1st"&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -3339,7 +3338,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B47" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -3372,7 +3371,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B52" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -3405,7 +3404,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B57" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>